<commit_message>
Acceptable format for the automation excel looks gucci AF i think
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,29 +1,399 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitmuck\MermaidExtractor\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9269BE6D-058D-4D49-BEB4-0F06DDE4E2EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
-  <si>
-    <t>Hello World</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="120">
+  <si>
+    <t xml:space="preserve">        title Timeline-Capstone-Part-B 
+</t>
+  </si>
+  <si>
+    <t>Activity Name</t>
+  </si>
+  <si>
+    <t>State Of The Activity</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Length Of Activity</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time-Allocated
+</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> weekNull</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 00                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 01                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 02                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 03                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 04                     </t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-08-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 05                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-08-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 06                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-08-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Break Week                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> weekBreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-08-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 07                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-09-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 08                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-09-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 09                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-09-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 10                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-09-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 11                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 12                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-10-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Week 13                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> week14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-10-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assesment-Tasks
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Completion Plan         </t>
+  </si>
+  <si>
+    <t>crit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after week3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7d </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Proffesional Practice &amp; Contribution </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after week12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Final Report </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after week11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Presentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after week13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software-Android
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Joining Protocol Re-Oriented </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after weekNull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Discovery Protocol Prototype </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Testing Joining Interaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">done </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Testing Discovery Interaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Software design on the fetching the metric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Verification on Joining &amp; Discovery Interaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Documentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Realtime Graph Adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Data Fetch from the API inside from the MCU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software-ESP8266
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Re-Oriented Joining Protocol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Discovery Protocol Integration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Integrating Joining and Discovery </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Design on a bounce diagram on metric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Software to send out metrics every 1 second </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Buffer Implementation to Record Humid and Temp Every Hour In The MCU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Buffer Implementation to Record Humid and Temp Wihtin the last two hours with resolution of 1 minutes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">active </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware-PCB
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Testing Relay </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Reoriented PCB Position </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Consulted PCB Position </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Finalizing PCB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCBFinalized</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-20</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Deploy PCB to production </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FinalizingPCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2018-07-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MidPoint PCB Deployment Days </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MidPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Assembly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Testing PCB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordering-Hardware
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Order and buy waterproof temperature sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after MidPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Order and buy enclosure for wireless sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Order and buy the input terminals </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holiday                     </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +430,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -106,7 +484,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -138,9 +516,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,6 +568,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -347,21 +761,855 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="94.06640625" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" t="s">
+        <v>114</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" t="s">
+        <v>114</v>
+      </c>
+      <c r="E73" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>